<commit_message>
modified:   datacleaning.py 	modified:   templates/Main_DataSet.xlsx 	new file:   templates/Main_DataSet_utf8.csv 	renamed:    templates/Main_DataSet_1000.csv -> templates/Main_DataSet_v1.csv 	new file:   templates/Main_DataSet_v2.csv 	new file:   templates/Main_DataSet_v3.csv
</commit_message>
<xml_diff>
--- a/templates/Main_DataSet.xlsx
+++ b/templates/Main_DataSet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Documents\~Dissertation Files\SystemPrototype\DissertationBackup\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Document\Dissertation Docs\DissertationBackup\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{69B25B86-583A-4BFF-9026-34C784A6A8BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EA877B0-F727-462D-AE8A-323C7574D846}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23475" yWindow="1470" windowWidth="22980" windowHeight="12195" tabRatio="398" xr2:uid="{9B11329D-6E49-4817-ADF2-FB61734A84BB}"/>
+    <workbookView xWindow="2172" yWindow="1656" windowWidth="17280" windowHeight="11256" tabRatio="398" xr2:uid="{9B11329D-6E49-4817-ADF2-FB61734A84BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Dataset" sheetId="2" r:id="rId1"/>
@@ -12689,17 +12689,17 @@
   </sheetPr>
   <dimension ref="A1:E2328"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23" style="2" customWidth="1"/>
     <col min="2" max="2" width="17" style="4" customWidth="1"/>
-    <col min="3" max="3" width="23" style="2" customWidth="1"/>
+    <col min="3" max="3" width="45.109375" style="2" customWidth="1"/>
     <col min="4" max="4" width="19.21875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="25.33203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="19.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
@@ -52744,23 +52744,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="7ed5eb0a-8eb0-42ba-991a-eddac6e1e9d2" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010033BBDAB3156DC548A1BABCE885DE578D" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ff07d59d3c987c72c6efa570b07b5008">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="7ed5eb0a-8eb0-42ba-991a-eddac6e1e9d2" xmlns:ns4="32f60cb4-90df-4d3d-848f-359bbc63c27f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="91cc909f0d04b8910aa11aa9d20930af" ns3:_="" ns4:_="">
     <xsd:import namespace="7ed5eb0a-8eb0-42ba-991a-eddac6e1e9d2"/>
@@ -53007,32 +52990,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1EA8B8EB-C9CF-4C78-A60B-A929121CC713}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="32f60cb4-90df-4d3d-848f-359bbc63c27f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="7ed5eb0a-8eb0-42ba-991a-eddac6e1e9d2"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C3F2B20-0969-466C-A124-05A4EF9BB641}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="7ed5eb0a-8eb0-42ba-991a-eddac6e1e9d2" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8D90301-1D8A-4812-992B-0C2A63668BA3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -53049,4 +53024,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C3F2B20-0969-466C-A124-05A4EF9BB641}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1EA8B8EB-C9CF-4C78-A60B-A929121CC713}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="32f60cb4-90df-4d3d-848f-359bbc63c27f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="7ed5eb0a-8eb0-42ba-991a-eddac6e1e9d2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>